<commit_message>
tweak of a test data
</commit_message>
<xml_diff>
--- a/inst/wyniki.xlsx
+++ b/inst/wyniki.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zajac/Dropbox/PEJK/ASIA/dane do testowania/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0EE354A-FD11-8A48-B150-781379C5C162}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ADC2FBF-F0CC-604B-9E95-3214724DC608}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1520" yWindow="1580" windowWidth="24280" windowHeight="14280" xr2:uid="{D26FE942-611F-194F-963B-EC166835772B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="26">
   <si>
     <t>pesel</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>S2-EKO-III</t>
+  </si>
+  <si>
+    <t>S1-STA</t>
   </si>
 </sst>
 </file>
@@ -452,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC8D06C5-8ECE-DF48-95D1-56176BA24442}">
-  <dimension ref="A1:I144"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132:H144"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="D145" sqref="D145:D174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3431,6 +3434,516 @@
         <v>1</v>
       </c>
     </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>98090100001</v>
+      </c>
+      <c r="B145" t="s">
+        <v>25</v>
+      </c>
+      <c r="D145">
+        <v>100</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
+      <c r="H145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>98090100002</v>
+      </c>
+      <c r="B146" t="s">
+        <v>25</v>
+      </c>
+      <c r="D146">
+        <v>99</v>
+      </c>
+      <c r="G146">
+        <v>1</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>98090100003</v>
+      </c>
+      <c r="B147" t="s">
+        <v>25</v>
+      </c>
+      <c r="D147">
+        <v>98</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>98090100004</v>
+      </c>
+      <c r="B148" t="s">
+        <v>25</v>
+      </c>
+      <c r="D148">
+        <v>97</v>
+      </c>
+      <c r="G148">
+        <v>1</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>98090100005</v>
+      </c>
+      <c r="B149" t="s">
+        <v>25</v>
+      </c>
+      <c r="D149">
+        <v>96</v>
+      </c>
+      <c r="G149">
+        <v>1</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>98090100006</v>
+      </c>
+      <c r="B150" t="s">
+        <v>25</v>
+      </c>
+      <c r="D150">
+        <v>95</v>
+      </c>
+      <c r="G150">
+        <v>1</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>98090100007</v>
+      </c>
+      <c r="B151" t="s">
+        <v>25</v>
+      </c>
+      <c r="D151">
+        <v>94</v>
+      </c>
+      <c r="G151">
+        <v>1</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>98090100008</v>
+      </c>
+      <c r="B152" t="s">
+        <v>25</v>
+      </c>
+      <c r="D152">
+        <v>93</v>
+      </c>
+      <c r="G152">
+        <v>1</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>98090100009</v>
+      </c>
+      <c r="B153" t="s">
+        <v>25</v>
+      </c>
+      <c r="D153">
+        <v>92</v>
+      </c>
+      <c r="G153">
+        <v>1</v>
+      </c>
+      <c r="H153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>98090100010</v>
+      </c>
+      <c r="B154" t="s">
+        <v>25</v>
+      </c>
+      <c r="D154">
+        <v>91</v>
+      </c>
+      <c r="G154">
+        <v>1</v>
+      </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>98090100011</v>
+      </c>
+      <c r="B155" t="s">
+        <v>25</v>
+      </c>
+      <c r="D155">
+        <v>90</v>
+      </c>
+      <c r="G155">
+        <v>1</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>98090100012</v>
+      </c>
+      <c r="B156" t="s">
+        <v>25</v>
+      </c>
+      <c r="D156">
+        <v>89</v>
+      </c>
+      <c r="G156">
+        <v>1</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>98090100013</v>
+      </c>
+      <c r="B157" t="s">
+        <v>25</v>
+      </c>
+      <c r="D157">
+        <v>88</v>
+      </c>
+      <c r="G157">
+        <v>1</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>98090100014</v>
+      </c>
+      <c r="B158" t="s">
+        <v>25</v>
+      </c>
+      <c r="D158">
+        <v>87</v>
+      </c>
+      <c r="G158">
+        <v>1</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>98090100015</v>
+      </c>
+      <c r="B159" t="s">
+        <v>25</v>
+      </c>
+      <c r="D159">
+        <v>86</v>
+      </c>
+      <c r="G159">
+        <v>1</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>98090100016</v>
+      </c>
+      <c r="B160" t="s">
+        <v>25</v>
+      </c>
+      <c r="D160">
+        <v>85</v>
+      </c>
+      <c r="G160">
+        <v>1</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>98090100017</v>
+      </c>
+      <c r="B161" t="s">
+        <v>25</v>
+      </c>
+      <c r="D161">
+        <v>84</v>
+      </c>
+      <c r="G161">
+        <v>1</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>98090100018</v>
+      </c>
+      <c r="B162" t="s">
+        <v>25</v>
+      </c>
+      <c r="D162">
+        <v>83</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
+      <c r="H162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>98090100019</v>
+      </c>
+      <c r="B163" t="s">
+        <v>25</v>
+      </c>
+      <c r="D163">
+        <v>82</v>
+      </c>
+      <c r="G163">
+        <v>1</v>
+      </c>
+      <c r="H163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>98090100020</v>
+      </c>
+      <c r="B164" t="s">
+        <v>25</v>
+      </c>
+      <c r="D164">
+        <v>81</v>
+      </c>
+      <c r="G164">
+        <v>0</v>
+      </c>
+      <c r="H164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>98090100021</v>
+      </c>
+      <c r="B165" t="s">
+        <v>25</v>
+      </c>
+      <c r="D165">
+        <v>80</v>
+      </c>
+      <c r="G165">
+        <v>0</v>
+      </c>
+      <c r="H165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>98090100022</v>
+      </c>
+      <c r="B166" t="s">
+        <v>25</v>
+      </c>
+      <c r="D166">
+        <v>79</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
+      <c r="H166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>98090100023</v>
+      </c>
+      <c r="B167" t="s">
+        <v>25</v>
+      </c>
+      <c r="D167">
+        <v>78</v>
+      </c>
+      <c r="G167">
+        <v>0</v>
+      </c>
+      <c r="H167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>98090100024</v>
+      </c>
+      <c r="B168" t="s">
+        <v>25</v>
+      </c>
+      <c r="D168">
+        <v>77</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
+      <c r="H168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>98090100025</v>
+      </c>
+      <c r="B169" t="s">
+        <v>25</v>
+      </c>
+      <c r="D169">
+        <v>76</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
+      <c r="H169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>98090100026</v>
+      </c>
+      <c r="B170" t="s">
+        <v>25</v>
+      </c>
+      <c r="D170">
+        <v>75</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
+      <c r="H170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>98090100027</v>
+      </c>
+      <c r="B171" t="s">
+        <v>25</v>
+      </c>
+      <c r="D171">
+        <v>74</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>98090100028</v>
+      </c>
+      <c r="B172" t="s">
+        <v>25</v>
+      </c>
+      <c r="D172">
+        <v>73</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>98090100029</v>
+      </c>
+      <c r="B173" t="s">
+        <v>25</v>
+      </c>
+      <c r="D173">
+        <v>72</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>98090100030</v>
+      </c>
+      <c r="B174" t="s">
+        <v>25</v>
+      </c>
+      <c r="D174">
+        <v>71</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
+      <c r="H174">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>